<commit_message>
Error corrections -Performance issue
</commit_message>
<xml_diff>
--- a/MLL_error_list.xlsx
+++ b/MLL_error_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harold\Documents\python\ARDUINO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC7C25F-0939-4881-94AE-A08764EC3D12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3694A01-36DF-4DB7-88B5-A05D91676D4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19080" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B7038BA0-A270-4BE5-8AAE-FFCEF6BA1D43}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="49">
   <si>
     <t>Beschreibung</t>
   </si>
@@ -162,6 +162,24 @@
   </si>
   <si>
     <t>needs some bigger changes, high risk</t>
+  </si>
+  <si>
+    <t>Performance very low</t>
+  </si>
+  <si>
+    <t>delay between ARDUINO message too high</t>
+  </si>
+  <si>
+    <t>2.30</t>
+  </si>
+  <si>
+    <t>Allow entry of individual portname (for MAC and LINUX users)</t>
+  </si>
+  <si>
+    <t>Improve group info handling</t>
+  </si>
+  <si>
+    <t>Springe zur zugehörigen Macroseite beim Acklicken einer LED in der LEDListe</t>
   </si>
 </sst>
 </file>
@@ -543,8 +561,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,7 +941,9 @@
       </c>
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
+      <c r="A16" s="5">
+        <v>1015</v>
+      </c>
       <c r="B16" s="7">
         <v>43951</v>
       </c>
@@ -943,7 +963,9 @@
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
+      <c r="A17" s="5">
+        <v>1016</v>
+      </c>
       <c r="B17" s="7">
         <v>43951</v>
       </c>
@@ -965,7 +987,9 @@
       </c>
     </row>
     <row r="18" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
+      <c r="A18" s="5">
+        <v>1017</v>
+      </c>
       <c r="B18" s="7">
         <v>43951</v>
       </c>
@@ -985,7 +1009,9 @@
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
+      <c r="A19" s="5">
+        <v>1018</v>
+      </c>
       <c r="B19" s="7">
         <v>43951</v>
       </c>
@@ -1007,7 +1033,9 @@
       </c>
     </row>
     <row r="20" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
+      <c r="A20" s="5">
+        <v>1019</v>
+      </c>
       <c r="B20" s="7">
         <v>43951</v>
       </c>
@@ -1021,48 +1049,105 @@
         <v>17</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="6"/>
+        <v>12</v>
+      </c>
       <c r="H20" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
+    <row r="21" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>1020</v>
+      </c>
+      <c r="B21" s="7">
+        <v>43952</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="22" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
+      <c r="A22" s="5">
+        <v>1021</v>
+      </c>
+      <c r="B22" s="7">
+        <v>43952</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="H22" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="23" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
+      <c r="A23" s="5">
+        <v>1032</v>
+      </c>
+      <c r="B23" s="7">
+        <v>43952</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+      <c r="H23" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>1033</v>
+      </c>
+      <c r="B24" s="7">
+        <v>43952</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
+      <c r="H24" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="25" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>

</xml_diff>

<commit_message>
In Haus-Makro eingebettete GasLights mit eigener DCC Adresse funktionieren jetzt richtig - siehe Beispiel
</commit_message>
<xml_diff>
--- a/MLL_error_list.xlsx
+++ b/MLL_error_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harold\Documents\python\ARDUINO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3694A01-36DF-4DB7-88B5-A05D91676D4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3C11E9-AD40-413A-AA6E-804C1D933E09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19080" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B7038BA0-A270-4BE5-8AAE-FFCEF6BA1D43}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="51">
   <si>
     <t>Beschreibung</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t>Springe zur zugehörigen Macroseite beim Acklicken einer LED in der LEDListe</t>
+  </si>
+  <si>
+    <t>Einbetten von GasLights mit eigener DCC Adresse Fehlerhaft</t>
+  </si>
+  <si>
+    <t>2.31</t>
   </si>
 </sst>
 </file>
@@ -562,7 +568,7 @@
   <dimension ref="A1:H78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,13 +1156,26 @@
       </c>
     </row>
     <row r="25" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+      <c r="A25" s="5">
+        <v>1034</v>
+      </c>
+      <c r="B25" s="7">
+        <v>43952</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
+      <c r="H25" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="26" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>

</xml_diff>

<commit_message>
Optimisation for small screens - Improved feedback from ARDUINO IDE
</commit_message>
<xml_diff>
--- a/MLL_error_list.xlsx
+++ b/MLL_error_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harold\Documents\python\ARDUINO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3C11E9-AD40-413A-AA6E-804C1D933E09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B095AC2-99DD-4862-B754-7B80FF80B1C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19080" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B7038BA0-A270-4BE5-8AAE-FFCEF6BA1D43}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="58">
   <si>
     <t>Beschreibung</t>
   </si>
@@ -186,6 +186,28 @@
   </si>
   <si>
     <t>2.31</t>
+  </si>
+  <si>
+    <t>2.32</t>
+  </si>
+  <si>
+    <t>Meldung von ARDUINO-Programm direkt in Echtzeit anzeigen</t>
+  </si>
+  <si>
+    <t>2.33</t>
+  </si>
+  <si>
+    <t>Optimierung für kleine Bildschirme (Scrollbalken für Proggen Fenster</t>
+  </si>
+  <si>
+    <t>Optimierung für kleine Bildschirme (Scrollbalken für ColorCheck und Configuration</t>
+  </si>
+  <si>
+    <t>In dem Makro Fire() ist ein kleiner "Bug" drin. Das Makro erfordert mindestens 3 RGB-LEDs, bei weniger werden bei mir alle LEDs genommen und angesteuert, egal was daran angeschlossen ist. 
+Hardi hat im Excel da ein Minimum von drei LEDs fest vorgegeben, weniger lässt das Excel nicht zu.</t>
+  </si>
+  <si>
+    <t>Das nächste ist mehr ein Wunsch. Kannst du den Button/ die Funktion "Blinken ein/aus" so gestalten, dass sich dieser das deaktivieren merkt oder z.B. den Modus wechselt von Blinken der LEDs auf alle anderen LEDs aus und nur die ausgewählten einschalten. Habe an zwei Extender-Platinen Relais angeschlossen und diese schalten sich beim Einstellen des Makros auf dieser Led laufend schnell ein und aus.</t>
   </si>
 </sst>
 </file>
@@ -567,8 +589,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,47 +1199,108 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+    <row r="26" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>1035</v>
+      </c>
+      <c r="B26" s="7">
+        <v>43953</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
+      <c r="H26" s="6" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="27" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+      <c r="A27" s="5">
+        <v>1036</v>
+      </c>
+      <c r="B27" s="7">
+        <v>43954</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-    </row>
-    <row r="28" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
+      <c r="H27" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>1037</v>
+      </c>
+      <c r="B28" s="7">
+        <v>43954</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-    </row>
-    <row r="29" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="H28" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>1038</v>
+      </c>
+      <c r="B29" s="7">
+        <v>43954</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
+    <row r="30" spans="1:8" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>1039</v>
+      </c>
+      <c r="B30" s="7">
+        <v>43954</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>

</xml_diff>

<commit_message>
Error in Servoadressing corrected - Automatic Comportlist update
</commit_message>
<xml_diff>
--- a/MLL_error_list.xlsx
+++ b/MLL_error_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harold\Documents\python\ARDUINO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B095AC2-99DD-4862-B754-7B80FF80B1C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79ED301-6A1E-4985-A96E-7C903428E0F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19080" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B7038BA0-A270-4BE5-8AAE-FFCEF6BA1D43}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="62">
   <si>
     <t>Beschreibung</t>
   </si>
@@ -208,6 +208,18 @@
   </si>
   <si>
     <t>Das nächste ist mehr ein Wunsch. Kannst du den Button/ die Funktion "Blinken ein/aus" so gestalten, dass sich dieser das deaktivieren merkt oder z.B. den Modus wechselt von Blinken der LEDs auf alle anderen LEDs aus und nur die ausgewählten einschalten. Habe an zwei Extender-Platinen Relais angeschlossen und diese schalten sich beim Einstellen des Makros auf dieser Led laufend schnell ein und aus.</t>
+  </si>
+  <si>
+    <t>3.35</t>
+  </si>
+  <si>
+    <t>Fehler bei Adressirung von Servos behoben</t>
+  </si>
+  <si>
+    <t>3.36</t>
+  </si>
+  <si>
+    <t>Automatisches Update der Comport-Liste, wenn der Einstellungstab geöffnet wird</t>
   </si>
 </sst>
 </file>
@@ -590,7 +602,7 @@
   <dimension ref="A1:H78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32:C33"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,7 +1295,9 @@
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
+      <c r="H29" s="6" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
@@ -1303,25 +1317,53 @@
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
+      <c r="H30" s="6" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
+      <c r="A31" s="5">
+        <v>1040</v>
+      </c>
+      <c r="B31" s="7">
+        <v>43955</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-    </row>
-    <row r="32" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
+      <c r="H31" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>1041</v>
+      </c>
+      <c r="B32" s="7">
+        <v>43955</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
+      <c r="H32" s="6" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="33" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>

</xml_diff>